<commit_message>
Pushing feature line, glue code and supporting code in other java files
</commit_message>
<xml_diff>
--- a/src/main/resources/Customer.xlsx
+++ b/src/main/resources/Customer.xlsx
@@ -26,13 +26,13 @@
     <t>Additional_Details</t>
   </si>
   <si>
-    <t>Burl</t>
+    <t>Bernardo</t>
   </si>
   <si>
-    <t>Kuhlman</t>
+    <t>Pfannerstill</t>
   </si>
   <si>
-    <t>lrrz53@gmail.com</t>
+    <t>htmt39@gmail.com</t>
   </si>
   <si>
     <t>Admin</t>

</xml_diff>

<commit_message>
Pushing code to take screenshots and to create word file by using CucumberHooks
</commit_message>
<xml_diff>
--- a/src/main/resources/Customer.xlsx
+++ b/src/main/resources/Customer.xlsx
@@ -26,13 +26,13 @@
     <t>Additional_Details</t>
   </si>
   <si>
-    <t>Bernardo</t>
+    <t>Asuncion</t>
   </si>
   <si>
-    <t>Pfannerstill</t>
+    <t>Koelpin</t>
   </si>
   <si>
-    <t>htmt39@gmail.com</t>
+    <t>buvc88@gmail.com</t>
   </si>
   <si>
     <t>Admin</t>

</xml_diff>

<commit_message>
Updated Xpath.yml file, arranged all the Xpath's in proper format and added corresponding code line to get Xpath from Xpath.yml file
</commit_message>
<xml_diff>
--- a/src/main/resources/Customer.xlsx
+++ b/src/main/resources/Customer.xlsx
@@ -26,13 +26,13 @@
     <t>Additional_Details</t>
   </si>
   <si>
-    <t>Asuncion</t>
+    <t>Bailey</t>
   </si>
   <si>
-    <t>Koelpin</t>
+    <t>Emmerich</t>
   </si>
   <si>
-    <t>buvc88@gmail.com</t>
+    <t>tbsf68@gmail.com</t>
   </si>
   <si>
     <t>Admin</t>

</xml_diff>

<commit_message>
Adding ChromeOption, EdgeOption properties and @FindBy annotation
</commit_message>
<xml_diff>
--- a/src/main/resources/Customer.xlsx
+++ b/src/main/resources/Customer.xlsx
@@ -26,13 +26,13 @@
     <t>Additional_Details</t>
   </si>
   <si>
-    <t>Bailey</t>
+    <t>Erasmo</t>
   </si>
   <si>
-    <t>Emmerich</t>
+    <t>Powlowski</t>
   </si>
   <si>
-    <t>tbsf68@gmail.com</t>
+    <t>abrh55@gmail.com</t>
   </si>
   <si>
     <t>Admin</t>

</xml_diff>